<commit_message>
updated total fertilizer production to 2023 - manual
</commit_message>
<xml_diff>
--- a/DataFeeds/E85.xlsx
+++ b/DataFeeds/E85.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meesam/Sandbox/Nutrien/Canpotex/DataFeeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA450A5-D9EB-4408-93F0-4E88BA4A0E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657629BE-62FC-4246-A3E2-8FF82D38BF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{43FC6F09-9C8B-471B-920F-EB1A8FB768A8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="19420" windowHeight="10420" xr2:uid="{43FC6F09-9C8B-471B-920F-EB1A8FB768A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -580,7 +580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,18 +588,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859F1B23-EA11-462E-8D38-DDC7EF09F573}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>36626</v>
       </c>
@@ -615,7 +615,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>36808</v>
       </c>
@@ -623,7 +623,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>37046</v>
       </c>
@@ -631,7 +631,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>37186</v>
       </c>
@@ -639,7 +639,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>37298</v>
       </c>
@@ -647,7 +647,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>37361</v>
       </c>
@@ -655,7 +655,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>37459</v>
       </c>
@@ -663,7 +663,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>37557</v>
       </c>
@@ -671,7 +671,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>37655</v>
       </c>
@@ -679,7 +679,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>37956</v>
       </c>
@@ -687,7 +687,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>38049</v>
       </c>
@@ -695,7 +695,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>38152</v>
       </c>
@@ -703,7 +703,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>38306</v>
       </c>
@@ -711,7 +711,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>38432</v>
       </c>
@@ -719,7 +719,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>38596</v>
       </c>
@@ -727,7 +727,7 @@
         <v>3.2105947398453307</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>38718</v>
       </c>
@@ -735,7 +735,7 @@
         <v>2.645566143056072</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>38861</v>
       </c>
@@ -743,7 +743,7 @@
         <v>3.2374457541634052</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>38964</v>
       </c>
@@ -751,7 +751,7 @@
         <v>2.806566651662191</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>39134</v>
       </c>
@@ -759,7 +759,7 @@
         <v>2.7946946934825565</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>39266</v>
       </c>
@@ -767,7 +767,7 @@
         <v>3.5049265839706401</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>39357</v>
       </c>
@@ -775,7 +775,7 @@
         <v>3.2003521058660405</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>39468</v>
       </c>
@@ -783,7 +783,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>39539</v>
       </c>
@@ -791,7 +791,7 @@
         <v>4.0599999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>39650</v>
       </c>
@@ -799,7 +799,7 @@
         <v>4.62</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>39723</v>
       </c>
@@ -807,7 +807,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>39825</v>
       </c>
@@ -815,7 +815,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>39904</v>
       </c>
@@ -823,7 +823,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>40014</v>
       </c>
@@ -831,7 +831,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>40102</v>
       </c>
@@ -839,7 +839,7 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>40197</v>
       </c>
@@ -847,7 +847,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>40270</v>
       </c>
@@ -855,7 +855,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>40371</v>
       </c>
@@ -863,7 +863,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>40455</v>
       </c>
@@ -871,7 +871,7 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>40567</v>
       </c>
@@ -879,7 +879,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>40634</v>
       </c>
@@ -887,7 +887,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>40738</v>
       </c>
@@ -895,7 +895,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>40816</v>
       </c>
@@ -903,7 +903,7 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>40921</v>
       </c>
@@ -911,7 +911,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>40998</v>
       </c>
@@ -919,7 +919,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>41103</v>
       </c>
@@ -927,7 +927,7 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>41180</v>
       </c>
@@ -935,7 +935,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>41284</v>
       </c>
@@ -943,7 +943,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>41362</v>
       </c>
@@ -951,7 +951,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>41467</v>
       </c>
@@ -959,7 +959,7 @@
         <v>4.57</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>41551</v>
       </c>
@@ -967,7 +967,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>41640</v>
       </c>
@@ -975,7 +975,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>41730</v>
       </c>
@@ -983,7 +983,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>41821</v>
       </c>
@@ -991,7 +991,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>41913</v>
       </c>
@@ -999,7 +999,7 @@
         <v>4.07</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>42005</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>42095</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>42186</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>42278</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>2.84</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>42370</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>42461</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>42552</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>42644</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>42736</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>42826</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>42917</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>43009</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>43101</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>43191</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>43282</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>43374</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>43466</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>43556</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>43647</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>43739</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>2.97</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>43831</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>43922</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>44013</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>44105</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>44197</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>44287</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>44378</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>44470</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>44562</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>44652</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="13">
         <v>44743</v>
       </c>
@@ -1248,13 +1248,49 @@
         <v>4.0066666666666668</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="13">
         <v>44835</v>
       </c>
       <c r="B82" s="14">
         <f>AVERAGE(B79:B81)</f>
         <v>4.1588888888888889</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="13">
+        <v>44927</v>
+      </c>
+      <c r="B83">
+        <f>_xlfn.FORECAST.LINEAR(A83,B76:B82,A76:A82)</f>
+        <v>4.5854049725218289</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="13">
+        <v>45017</v>
+      </c>
+      <c r="B84">
+        <f t="shared" ref="B84:B86" si="0">_xlfn.FORECAST.LINEAR(A84,B78:B83,A78:A83)</f>
+        <v>4.6721817647136135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="13">
+        <v>45108</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="0"/>
+        <v>4.7265063871419244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="13">
+        <v>45200</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="0"/>
+        <v>4.7641825467928314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>